<commit_message>
update calibration PD & Macro
Update Calibratoin PD input to include Segment
Add Calibration PD CommsCons Result
Fix order bug on Macros input summary
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Calibration/CalibrationInput_PD_CR_DR.xlsx
+++ b/angular/src/assets/sampleFiles/Calibration/CalibrationInput_PD_CR_DR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\ETI_ECL_Engine\angular\src\assets\sampleFiles\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82665A5-23E5-4728-AD5E-106E9A1DE316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8068D2E0-4409-46C9-99C9-AADAC8E5FD0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="3960" windowWidth="18330" windowHeight="11205" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="27" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>Customer_No</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>SEGMENT</t>
+  </si>
+  <si>
+    <t>CONSUMER</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B1E5E2-FB3A-4804-B949-E2061B45DF3F}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1055,7 @@
     <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1083,8 +1089,11 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1103,8 +1112,11 @@
       <c r="K2" s="4">
         <v>201603</v>
       </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1123,8 +1135,11 @@
       <c r="K3" s="4">
         <v>201603</v>
       </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1143,8 +1158,11 @@
       <c r="K4" s="4">
         <v>201603</v>
       </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1163,8 +1181,11 @@
       <c r="K5" s="4">
         <v>201603</v>
       </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1183,8 +1204,11 @@
       <c r="K6" s="4">
         <v>201603</v>
       </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1203,8 +1227,11 @@
       <c r="K7" s="4">
         <v>201603</v>
       </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1223,8 +1250,11 @@
       <c r="K8" s="4">
         <v>201603</v>
       </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1243,8 +1273,11 @@
       <c r="K9" s="4">
         <v>201603</v>
       </c>
+      <c r="L9" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1263,8 +1296,11 @@
       <c r="K10" s="4">
         <v>201603</v>
       </c>
+      <c r="L10" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>